<commit_message>
Update Billings, Plan de trabajo.xlsx
</commit_message>
<xml_diff>
--- a/Billings, Plan de trabajo.xlsx
+++ b/Billings, Plan de trabajo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29301"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://silicomfr-my.sharepoint.com/personal/lmejia_ext_neverhack_com/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71D29FC9-A26E-49C3-BE46-646E540F7A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1146" documentId="8_{C733FD18-DD95-4636-B138-AC785202E5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A270207-61D0-4226-A2CE-33C12E21214D}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5BAA692F-6A36-452E-95B2-09A7D7FC7E8C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="58">
   <si>
     <t>Plan de trabajo Billings</t>
   </si>
@@ -51,7 +51,7 @@
     <t>Diseño de componentes</t>
   </si>
   <si>
-    <t xml:space="preserve">Definicion </t>
+    <t xml:space="preserve">% avance </t>
   </si>
   <si>
     <t>Inicio</t>
@@ -72,9 +72,6 @@
     <t>SNTDR_BIL_BP_PROCESA_OPERACIONES</t>
   </si>
   <si>
-    <t>Falta archivo Flag y tablas catalogos</t>
-  </si>
-  <si>
     <t>SNTDR_BIL_BP_PROCESA_OPERACIONES_SPLIT</t>
   </si>
   <si>
@@ -84,13 +81,16 @@
     <t>SNTDR_BIL_MAP_PROCESA_OPERACIONES_SERV_SPLIT</t>
   </si>
   <si>
+    <t>SNTDR_BIL_MAP_SPLIT</t>
+  </si>
+  <si>
     <t>Conteo diario</t>
   </si>
   <si>
     <t>SNTDR_BIL_BP_CONTEO_DIARIO</t>
   </si>
   <si>
-    <t xml:space="preserve">Falta de tablas definitivas </t>
+    <t>Homologacion de tablas (Ejemplo NUM_ACCOUNT Varchar 34)</t>
   </si>
   <si>
     <t>SNTDR_BIL_BP_CONTEO_DIARIO_POR_CLIENTE</t>
@@ -99,21 +99,18 @@
     <t>SNTDR_BIL_MAP_CONTEO_DIARIO_FILTRAR_TRS_SRV</t>
   </si>
   <si>
-    <t>Falta de tablas definitivas  y ¿Va a ser el mismo Pool que el de H2H o va a ser uno para Billing?</t>
-  </si>
-  <si>
     <t>SNTDR_BIL_MAP_CONTEO_DIARIO_ACUMULADO</t>
   </si>
   <si>
-    <t>Falta de tablas definitivas y ¿Va a ser el mismo Pool que el de H2H o va a ser uno para Billing?</t>
-  </si>
-  <si>
     <t>Calculo</t>
   </si>
   <si>
     <t>SNTDR_BIL_BP_CALCULO_COMISIONES_MAIN</t>
   </si>
   <si>
+    <t>Falta API cambio de divisa</t>
+  </si>
+  <si>
     <t>SNTDR_BIL_BP_CALCULO_COMISIONES_POR _CLIENTE</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>SNTDR_BIL_MAP_CALCULO_COMISIONES_FECHA</t>
   </si>
   <si>
-    <t>Falta catalogo de fechas, faltan tablas definitivas y ¿Va a ser el mismo Pool que el de H2H o va a ser uno para Billing?</t>
-  </si>
-  <si>
     <t>Cobro</t>
   </si>
   <si>
@@ -153,10 +147,19 @@
     <t>Reportes</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
-    <t>Los reportes no han sido definidos</t>
+    <t>SNTDR_BIL_BP_EXTRACT_COMISI_REPORT_DATE</t>
+  </si>
+  <si>
+    <t>SNTDR_BIL_BP_EXTRACT_COMISI_REPORT_INFO</t>
+  </si>
+  <si>
+    <t>Faltan APIs, definir el idioma en tablas y ejemplos PDF</t>
+  </si>
+  <si>
+    <t>SNTDR_BIL_BP_GENERA_COMISI_REPORT</t>
+  </si>
+  <si>
+    <t>SNTDR_BIL_MAP_COMISI_REPORT_TRANSFORM</t>
   </si>
   <si>
     <t>Documentación Diseño</t>
@@ -165,31 +168,19 @@
     <t>Construcción de componentes</t>
   </si>
   <si>
-    <t>Desarrollo de componentes en proceso y sin definición pendiente</t>
-  </si>
-  <si>
-    <t>Desarrollo de componentes en proceso con tablas temporales a falta de tablas definitivas y falta definir archivo Flag</t>
-  </si>
-  <si>
-    <t>Se  termino la construcción con tablas temporales, se esperan tablas definitivas para validar y cerrar la tarea</t>
-  </si>
-  <si>
-    <t>Desarrollo de componentes en proceso con tablas temporales a falta de tablas definitivas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desarrollo de componentes en proceso con tablas temporales a falta de tablas definitivas </t>
-  </si>
-  <si>
-    <t>Desarrollo de componentes en proceso con tablas temporales a falta de tablas definitivas y ¿Va a ser el mismo Pool que el de H2H o va a ser uno para Billing?</t>
-  </si>
-  <si>
-    <t>Desarrollo de componentes en proceso con tablas temporales a falta de tablas definitivas  y ¿Va a ser el mismo Pool que el de H2H o va a ser uno para Billing?</t>
-  </si>
-  <si>
-    <t>El plataformado de la maquina de Montse esta en curso, se ha iniciado con la construcción de mapas y queries</t>
+    <t>Desarrollo de componentes en proceso</t>
+  </si>
+  <si>
+    <t>Desarrollo de componentes en proceso y Cifras de control</t>
+  </si>
+  <si>
+    <t>Homologacion de tablas (NUM_ACCOUNT Varchar 34)</t>
   </si>
   <si>
     <t>SNTDR_BIL_MAP_CALCULO_COMISIONES</t>
+  </si>
+  <si>
+    <t>Falta APIs, definir el idioma en tablas y ejemplos PDF</t>
   </si>
   <si>
     <t>Documentación Construcción (Matriz Casos de prueba y FOR-DES-502)</t>
@@ -251,7 +242,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -267,6 +258,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -324,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -355,6 +352,8 @@
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -362,7 +361,64 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="32">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -974,10 +1030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D938FF59-382B-482E-B7AD-44B2F1E5CDDE}">
-  <dimension ref="A1:T59"/>
+  <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -990,7 +1046,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="14"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1034,15 +1090,15 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="14" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="14"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1123,7 +1179,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="6">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="C6" s="7">
         <v>45894</v>
@@ -1134,9 +1190,7 @@
       <c r="E6" s="7">
         <v>45895</v>
       </c>
-      <c r="F6" s="7">
-        <v>45895</v>
-      </c>
+      <c r="F6" s="3"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:20">
@@ -1144,7 +1198,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="6">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="C7" s="7">
         <v>45894</v>
@@ -1155,10 +1209,8 @@
       <c r="E7" s="7">
         <v>45895</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="2"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1175,10 +1227,10 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="6">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="C8" s="7">
         <v>45895</v>
@@ -1189,9 +1241,7 @@
       <c r="E8" s="7">
         <v>45895</v>
       </c>
-      <c r="F8" s="7">
-        <v>45895</v>
-      </c>
+      <c r="F8" s="3"/>
       <c r="G8" s="2"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1209,9 +1259,9 @@
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="6">
+        <v>12</v>
+      </c>
+      <c r="B9" s="15">
         <v>1</v>
       </c>
       <c r="C9" s="7">
@@ -1243,9 +1293,9 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="6">
+        <v>13</v>
+      </c>
+      <c r="B10" s="15">
         <v>1</v>
       </c>
       <c r="C10" s="7">
@@ -1276,14 +1326,24 @@
       <c r="T10" s="1"/>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="A11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="15">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10">
+        <v>45915</v>
+      </c>
+      <c r="D11" s="7">
+        <v>45918</v>
+      </c>
+      <c r="E11" s="10">
+        <v>45915</v>
+      </c>
+      <c r="F11" s="7">
+        <v>45918</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1300,25 +1360,15 @@
       <c r="T11" s="1"/>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="C12" s="7">
-        <v>45894</v>
-      </c>
-      <c r="D12" s="7">
-        <v>45894</v>
-      </c>
-      <c r="E12" s="7">
-        <v>45896</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="A12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1335,7 +1385,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13" s="6">
         <v>0.9</v>
@@ -1369,23 +1419,23 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="6">
-        <v>0.99</v>
+        <v>0.9</v>
       </c>
       <c r="C14" s="7">
-        <v>45895</v>
+        <v>45894</v>
       </c>
       <c r="D14" s="7">
-        <v>45895</v>
+        <v>45894</v>
       </c>
       <c r="E14" s="7">
         <v>45896</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1403,10 +1453,10 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" s="6">
-        <v>0.99</v>
+        <v>0.9</v>
       </c>
       <c r="C15" s="7">
         <v>45895</v>
@@ -1419,7 +1469,7 @@
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1436,15 +1486,25 @@
       <c r="T15" s="1"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="A16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="C16" s="7">
+        <v>45895</v>
+      </c>
+      <c r="D16" s="7">
+        <v>45895</v>
+      </c>
+      <c r="E16" s="7">
+        <v>45896</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1460,25 +1520,15 @@
       <c r="T16" s="1"/>
     </row>
     <row r="17" spans="1:20">
-      <c r="A17" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="C17" s="7">
-        <v>45894</v>
-      </c>
-      <c r="D17" s="7">
-        <v>45894</v>
-      </c>
-      <c r="E17" s="7">
-        <v>45901</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="A17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1495,10 +1545,10 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18" s="6">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="C18" s="7">
         <v>45894</v>
@@ -1511,7 +1561,7 @@
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1529,7 +1579,7 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B19" s="6">
         <v>0.9</v>
@@ -1544,9 +1594,7 @@
         <v>45901</v>
       </c>
       <c r="F19" s="7"/>
-      <c r="G19" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="G19" s="2"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1563,24 +1611,22 @@
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B20" s="6">
         <v>0.9</v>
       </c>
       <c r="C20" s="7">
-        <v>45895</v>
+        <v>45894</v>
       </c>
       <c r="D20" s="7">
-        <v>45895</v>
+        <v>45894</v>
       </c>
       <c r="E20" s="7">
         <v>45901</v>
       </c>
       <c r="F20" s="7"/>
-      <c r="G20" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="G20" s="2"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1597,7 +1643,7 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B21" s="6">
         <v>0.9</v>
@@ -1612,9 +1658,7 @@
         <v>45901</v>
       </c>
       <c r="F21" s="7"/>
-      <c r="G21" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="G21" s="2"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -1630,14 +1674,22 @@
       <c r="T21" s="1"/>
     </row>
     <row r="22" spans="1:20">
-      <c r="A22" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="A22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="C22" s="7">
+        <v>45895</v>
+      </c>
+      <c r="D22" s="7">
+        <v>45895</v>
+      </c>
+      <c r="E22" s="7">
+        <v>45901</v>
+      </c>
+      <c r="F22" s="7"/>
       <c r="G22" s="2"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1654,25 +1706,15 @@
       <c r="T22" s="1"/>
     </row>
     <row r="23" spans="1:20">
-      <c r="A23" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="6">
-        <v>0.9</v>
-      </c>
-      <c r="C23" s="7">
-        <v>45894</v>
-      </c>
-      <c r="D23" s="7">
-        <v>45894</v>
-      </c>
-      <c r="E23" s="7">
-        <v>45905</v>
-      </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="A23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1689,7 +1731,7 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B24" s="6">
         <v>0.9</v>
@@ -1704,9 +1746,7 @@
         <v>45905</v>
       </c>
       <c r="F24" s="7"/>
-      <c r="G24" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="G24" s="2"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1723,7 +1763,7 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B25" s="6">
         <v>0.9</v>
@@ -1737,10 +1777,8 @@
       <c r="E25" s="7">
         <v>45905</v>
       </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="2"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1757,24 +1795,22 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B26" s="6">
         <v>0.9</v>
       </c>
       <c r="C26" s="7">
-        <v>45895</v>
+        <v>45894</v>
       </c>
       <c r="D26" s="7">
-        <v>45895</v>
+        <v>45894</v>
       </c>
       <c r="E26" s="7">
         <v>45905</v>
       </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="2"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1791,7 +1827,7 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B27" s="6">
         <v>0.9</v>
@@ -1805,10 +1841,8 @@
       <c r="E27" s="7">
         <v>45905</v>
       </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="2"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1825,7 +1859,7 @@
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B28" s="6">
         <v>0.9</v>
@@ -1839,10 +1873,8 @@
       <c r="E28" s="7">
         <v>45905</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="2"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -1858,19 +1890,23 @@
       <c r="T28" s="1"/>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="12" t="s">
-        <v>39</v>
-      </c>
+      <c r="A29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="C29" s="7">
+        <v>45895</v>
+      </c>
+      <c r="D29" s="7">
+        <v>45895</v>
+      </c>
+      <c r="E29" s="7">
+        <v>45905</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="2"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -1887,20 +1923,14 @@
     </row>
     <row r="30" spans="1:20">
       <c r="A30" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="6">
-        <v>0</v>
-      </c>
-      <c r="C30" s="7">
-        <v>45947</v>
-      </c>
-      <c r="D30" s="7">
-        <v>45947</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="12"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -1916,15 +1946,23 @@
       <c r="T30" s="1"/>
     </row>
     <row r="31" spans="1:20">
-      <c r="A31" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
+      <c r="A31" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C31" s="7">
+        <v>45918</v>
+      </c>
+      <c r="D31" s="7">
+        <v>45923</v>
+      </c>
+      <c r="E31" s="7">
+        <v>45918</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="12"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -1940,15 +1978,25 @@
       <c r="T31" s="1"/>
     </row>
     <row r="32" spans="1:20">
-      <c r="A32" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="A32" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C32" s="7">
+        <v>45918</v>
+      </c>
+      <c r="D32" s="7">
+        <v>45923</v>
+      </c>
+      <c r="E32" s="7">
+        <v>45918</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -1965,23 +2013,23 @@
     </row>
     <row r="33" spans="1:20">
       <c r="A33" s="5" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B33" s="6">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="C33" s="7">
-        <v>45897</v>
+        <v>45918</v>
       </c>
       <c r="D33" s="7">
-        <v>45897</v>
+        <v>45923</v>
       </c>
       <c r="E33" s="7">
-        <v>45902</v>
+        <v>45918</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -1999,24 +2047,22 @@
     </row>
     <row r="34" spans="1:20">
       <c r="A34" s="5" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B34" s="6">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="C34" s="7">
-        <v>45897</v>
+        <v>45918</v>
       </c>
       <c r="D34" s="7">
-        <v>45908</v>
+        <v>45923</v>
       </c>
       <c r="E34" s="7">
-        <v>45904</v>
+        <v>45918</v>
       </c>
       <c r="F34" s="7"/>
-      <c r="G34" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="G34" s="12"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -2032,25 +2078,21 @@
       <c r="T34" s="1"/>
     </row>
     <row r="35" spans="1:20">
-      <c r="A35" s="5" t="s">
-        <v>12</v>
+      <c r="A35" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="B35" s="6">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="C35" s="7">
-        <v>45897</v>
+        <v>45947</v>
       </c>
       <c r="D35" s="7">
-        <v>45897</v>
-      </c>
-      <c r="E35" s="7">
-        <v>45908</v>
-      </c>
-      <c r="F35" s="7"/>
-      <c r="G35" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>45947</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="2"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -2066,25 +2108,15 @@
       <c r="T35" s="1"/>
     </row>
     <row r="36" spans="1:20">
-      <c r="A36" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="C36" s="7">
-        <v>45897</v>
-      </c>
-      <c r="D36" s="7">
-        <v>45908</v>
-      </c>
-      <c r="E36" s="7">
-        <v>45908</v>
-      </c>
-      <c r="F36" s="7"/>
-      <c r="G36" s="2" t="s">
+      <c r="A36" s="9" t="s">
         <v>42</v>
       </c>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -2100,25 +2132,15 @@
       <c r="T36" s="1"/>
     </row>
     <row r="37" spans="1:20">
-      <c r="A37" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="C37" s="7">
-        <v>45897</v>
-      </c>
-      <c r="D37" s="7">
-        <v>45908</v>
-      </c>
-      <c r="E37" s="10">
-        <v>45909</v>
-      </c>
-      <c r="F37" s="7"/>
-      <c r="G37" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="A37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -2134,15 +2156,25 @@
       <c r="T37" s="1"/>
     </row>
     <row r="38" spans="1:20">
-      <c r="A38" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+      <c r="A38" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="C38" s="7">
+        <v>45897</v>
+      </c>
+      <c r="D38" s="7">
+        <v>45897</v>
+      </c>
+      <c r="E38" s="7">
+        <v>45902</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -2159,23 +2191,23 @@
     </row>
     <row r="39" spans="1:20">
       <c r="A39" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B39" s="6">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="C39" s="7">
         <v>45897</v>
       </c>
       <c r="D39" s="7">
-        <v>45898</v>
+        <v>45908</v>
       </c>
       <c r="E39" s="7">
-        <v>45902</v>
+        <v>45904</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -2193,23 +2225,23 @@
     </row>
     <row r="40" spans="1:20">
       <c r="A40" s="5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B40" s="6">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="C40" s="7">
         <v>45897</v>
       </c>
       <c r="D40" s="7">
-        <v>45898</v>
+        <v>45897</v>
       </c>
       <c r="E40" s="7">
-        <v>45902</v>
+        <v>45908</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -2227,23 +2259,23 @@
     </row>
     <row r="41" spans="1:20">
       <c r="A41" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B41" s="6">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="C41" s="7">
-        <v>45898</v>
+        <v>45897</v>
       </c>
       <c r="D41" s="7">
-        <v>45905</v>
+        <v>45908</v>
       </c>
       <c r="E41" s="7">
         <v>45908</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -2261,21 +2293,23 @@
     </row>
     <row r="42" spans="1:20">
       <c r="A42" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B42" s="6">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="C42" s="7">
-        <v>45898</v>
+        <v>45897</v>
       </c>
       <c r="D42" s="7">
-        <v>45905</v>
-      </c>
-      <c r="E42" s="7"/>
+        <v>45908</v>
+      </c>
+      <c r="E42" s="10">
+        <v>45909</v>
+      </c>
       <c r="F42" s="7"/>
       <c r="G42" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -2292,14 +2326,24 @@
       <c r="T42" s="1"/>
     </row>
     <row r="43" spans="1:20">
-      <c r="A43" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
+      <c r="A43" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="6">
+        <v>1</v>
+      </c>
+      <c r="C43" s="10">
+        <v>45915</v>
+      </c>
+      <c r="D43" s="7">
+        <v>45918</v>
+      </c>
+      <c r="E43" s="10">
+        <v>45915</v>
+      </c>
+      <c r="F43" s="7">
+        <v>45918</v>
+      </c>
       <c r="G43" s="2"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -2316,25 +2360,15 @@
       <c r="T43" s="1"/>
     </row>
     <row r="44" spans="1:20">
-      <c r="A44" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B44" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="C44" s="7">
-        <v>45897</v>
-      </c>
-      <c r="D44" s="7">
-        <v>45902</v>
-      </c>
-      <c r="E44" s="7">
-        <v>45902</v>
-      </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="A44" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="7"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -2351,23 +2385,23 @@
     </row>
     <row r="45" spans="1:20">
       <c r="A45" s="5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B45" s="6">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="C45" s="7">
-        <v>45902</v>
+        <v>45897</v>
       </c>
       <c r="D45" s="7">
-        <v>45904</v>
+        <v>45898</v>
       </c>
       <c r="E45" s="7">
         <v>45902</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -2385,23 +2419,23 @@
     </row>
     <row r="46" spans="1:20">
       <c r="A46" s="5" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="B46" s="6">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="C46" s="7">
-        <v>45904</v>
+        <v>45897</v>
       </c>
       <c r="D46" s="7">
-        <v>45910</v>
+        <v>45898</v>
       </c>
       <c r="E46" s="7">
-        <v>45905</v>
+        <v>45902</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -2419,21 +2453,23 @@
     </row>
     <row r="47" spans="1:20">
       <c r="A47" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B47" s="6">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="C47" s="7">
-        <v>45910</v>
+        <v>45898</v>
       </c>
       <c r="D47" s="7">
-        <v>45915</v>
-      </c>
-      <c r="E47" s="7"/>
+        <v>45905</v>
+      </c>
+      <c r="E47" s="7">
+        <v>45908</v>
+      </c>
       <c r="F47" s="7"/>
       <c r="G47" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -2451,23 +2487,23 @@
     </row>
     <row r="48" spans="1:20">
       <c r="A48" s="5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B48" s="6">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="C48" s="7">
-        <v>45915</v>
+        <v>45898</v>
       </c>
       <c r="D48" s="7">
-        <v>45918</v>
+        <v>45905</v>
       </c>
       <c r="E48" s="7">
-        <v>45909</v>
+        <v>45911</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -2485,7 +2521,7 @@
     </row>
     <row r="49" spans="1:20">
       <c r="A49" s="4" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="2"/>
@@ -2509,23 +2545,23 @@
     </row>
     <row r="50" spans="1:20">
       <c r="A50" s="5" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B50" s="6">
-        <v>0.75</v>
+        <v>0.2</v>
       </c>
       <c r="C50" s="7">
         <v>45897</v>
       </c>
       <c r="D50" s="7">
-        <v>45903</v>
+        <v>45902</v>
       </c>
       <c r="E50" s="7">
-        <v>45904</v>
+        <v>45902</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -2543,23 +2579,23 @@
     </row>
     <row r="51" spans="1:20">
       <c r="A51" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B51" s="6">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="C51" s="7">
         <v>45902</v>
       </c>
       <c r="D51" s="7">
-        <v>45905</v>
+        <v>45904</v>
       </c>
       <c r="E51" s="7">
-        <v>45904</v>
+        <v>45902</v>
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
@@ -2577,23 +2613,23 @@
     </row>
     <row r="52" spans="1:20">
       <c r="A52" s="5" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B52" s="6">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="C52" s="7">
+        <v>45904</v>
+      </c>
+      <c r="D52" s="7">
+        <v>45910</v>
+      </c>
+      <c r="E52" s="7">
         <v>45905</v>
-      </c>
-      <c r="D52" s="7">
-        <v>45908</v>
-      </c>
-      <c r="E52" s="7">
-        <v>45904</v>
       </c>
       <c r="F52" s="7"/>
       <c r="G52" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
@@ -2611,21 +2647,21 @@
     </row>
     <row r="53" spans="1:20">
       <c r="A53" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B53" s="6">
         <v>0</v>
       </c>
       <c r="C53" s="7">
-        <v>45908</v>
+        <v>45910</v>
       </c>
       <c r="D53" s="7">
-        <v>45910</v>
+        <v>45915</v>
       </c>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
       <c r="G53" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -2643,23 +2679,23 @@
     </row>
     <row r="54" spans="1:20">
       <c r="A54" s="5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B54" s="6">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="C54" s="7">
-        <v>45910</v>
+        <v>45915</v>
       </c>
       <c r="D54" s="7">
-        <v>45912</v>
+        <v>45918</v>
       </c>
       <c r="E54" s="7">
-        <v>45904</v>
+        <v>45909</v>
       </c>
       <c r="F54" s="7"/>
       <c r="G54" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
@@ -2676,23 +2712,15 @@
       <c r="T54" s="1"/>
     </row>
     <row r="55" spans="1:20">
-      <c r="A55" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B55" s="6">
-        <v>0</v>
-      </c>
-      <c r="C55" s="7">
-        <v>45915</v>
-      </c>
-      <c r="D55" s="7">
-        <v>45918</v>
-      </c>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="A55" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B55" s="7"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
@@ -2708,17 +2736,25 @@
       <c r="T55" s="1"/>
     </row>
     <row r="56" spans="1:20">
-      <c r="A56" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
+      <c r="A56" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="C56" s="7">
+        <v>45897</v>
+      </c>
+      <c r="D56" s="7">
+        <v>45903</v>
+      </c>
+      <c r="E56" s="7">
+        <v>45904</v>
+      </c>
+      <c r="F56" s="7"/>
+      <c r="G56" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
@@ -2734,21 +2770,25 @@
       <c r="T56" s="1"/>
     </row>
     <row r="57" spans="1:20">
-      <c r="A57" s="4" t="s">
-        <v>51</v>
+      <c r="A57" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="B57" s="6">
-        <v>0</v>
-      </c>
-      <c r="C57" s="10">
-        <v>45947</v>
-      </c>
-      <c r="D57" s="10">
-        <v>45947</v>
-      </c>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="C57" s="7">
+        <v>45902</v>
+      </c>
+      <c r="D57" s="7">
+        <v>45905</v>
+      </c>
+      <c r="E57" s="7">
+        <v>45904</v>
+      </c>
+      <c r="F57" s="7"/>
+      <c r="G57" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
@@ -2765,20 +2805,24 @@
     </row>
     <row r="58" spans="1:20">
       <c r="A58" s="5" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B58" s="6">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="C58" s="7">
-        <v>45943</v>
+        <v>45905</v>
       </c>
       <c r="D58" s="7">
-        <v>45943</v>
-      </c>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
+        <v>45908</v>
+      </c>
+      <c r="E58" s="7">
+        <v>45904</v>
+      </c>
+      <c r="F58" s="7"/>
+      <c r="G58" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
@@ -2794,166 +2838,509 @@
       <c r="T58" s="1"/>
     </row>
     <row r="59" spans="1:20">
-      <c r="A59" s="8" t="s">
-        <v>53</v>
+      <c r="A59" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="B59" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C59" s="7">
+        <v>45908</v>
+      </c>
+      <c r="D59" s="7">
+        <v>45910</v>
+      </c>
+      <c r="E59" s="7">
+        <v>45917</v>
+      </c>
+      <c r="F59" s="7"/>
+      <c r="G59" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="1"/>
+      <c r="T59" s="1"/>
+    </row>
+    <row r="60" spans="1:20">
+      <c r="A60" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B60" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="C60" s="7">
+        <v>45910</v>
+      </c>
+      <c r="D60" s="7">
+        <v>45912</v>
+      </c>
+      <c r="E60" s="7">
+        <v>45904</v>
+      </c>
+      <c r="F60" s="7"/>
+      <c r="G60" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="1"/>
+      <c r="T60" s="1"/>
+    </row>
+    <row r="61" spans="1:20">
+      <c r="A61" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B61" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C61" s="7">
+        <v>45915</v>
+      </c>
+      <c r="D61" s="7">
+        <v>45918</v>
+      </c>
+      <c r="E61" s="7">
+        <v>45917</v>
+      </c>
+      <c r="F61" s="7"/>
+      <c r="G61" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
+      <c r="S61" s="1"/>
+      <c r="T61" s="1"/>
+    </row>
+    <row r="62" spans="1:20">
+      <c r="A62" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B62" s="13"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1"/>
+      <c r="S62" s="1"/>
+      <c r="T62" s="1"/>
+    </row>
+    <row r="63" spans="1:20">
+      <c r="A63" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B63" s="6">
         <v>0</v>
       </c>
-      <c r="C59" s="7">
+      <c r="C63" s="7">
+        <v>45923</v>
+      </c>
+      <c r="D63" s="7">
+        <v>45932</v>
+      </c>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
+      <c r="T63" s="1"/>
+    </row>
+    <row r="64" spans="1:20">
+      <c r="A64" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B64" s="6">
+        <v>0</v>
+      </c>
+      <c r="C64" s="7">
+        <v>45923</v>
+      </c>
+      <c r="D64" s="7">
+        <v>45932</v>
+      </c>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="1"/>
+      <c r="T64" s="1"/>
+    </row>
+    <row r="65" spans="1:20">
+      <c r="A65" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B65" s="6">
+        <v>0</v>
+      </c>
+      <c r="C65" s="7">
+        <v>45923</v>
+      </c>
+      <c r="D65" s="7">
+        <v>45932</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+      <c r="S65" s="1"/>
+      <c r="T65" s="1"/>
+    </row>
+    <row r="66" spans="1:20">
+      <c r="A66" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B66" s="6">
+        <v>0</v>
+      </c>
+      <c r="C66" s="7">
+        <v>45923</v>
+      </c>
+      <c r="D66" s="7">
+        <v>45932</v>
+      </c>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="1"/>
+    </row>
+    <row r="67" spans="1:20">
+      <c r="A67" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B67" s="6">
+        <v>0</v>
+      </c>
+      <c r="C67" s="10">
+        <v>45947</v>
+      </c>
+      <c r="D67" s="10">
+        <v>45947</v>
+      </c>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="1"/>
+    </row>
+    <row r="68" spans="1:20">
+      <c r="A68" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B68" s="6">
+        <v>0</v>
+      </c>
+      <c r="C68" s="7">
         <v>45943</v>
       </c>
-      <c r="D59" s="7">
+      <c r="D68" s="7">
         <v>45943</v>
       </c>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="1"/>
+      <c r="T68" s="1"/>
+    </row>
+    <row r="69" spans="1:20">
+      <c r="A69" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B69" s="6">
+        <v>0</v>
+      </c>
+      <c r="C69" s="7">
+        <v>45943</v>
+      </c>
+      <c r="D69" s="7">
+        <v>45943</v>
+      </c>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
   </mergeCells>
-  <conditionalFormatting sqref="B6:B10 B12:B15 B33:B37 B17:B21 B39:B42 B44:B48 B50:B55 B23:B28">
-    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+  <conditionalFormatting sqref="B38:B43 B45:B48 B50:B54 B56:B61 B24:B29 B13:B16 B6:B11 B18:B22">
+    <cfRule type="cellIs" dxfId="31" priority="56" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:B10 A12:B15 A11 A33:B37 A17:B21 A16 A22 A29:A32 A39:B42 A38 A44:B48 A43 A50:B55 A49 A56:A59 A23:B28">
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
+  <conditionalFormatting sqref="A38:B43 A17 A23 A45:B48 A44 A50:B54 A49 A56:B61 A55 A24:B29 A13:B16 A11:A12 A6:B11 A18:B22 A30:A37 A62:A69">
+    <cfRule type="cellIs" dxfId="30" priority="55" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:B10 B12:B15 B33:B37 B17:B21 B39:B42 B44:B48 B50:B55 B23:B28">
-    <cfRule type="cellIs" dxfId="23" priority="24" operator="between">
-      <formula>$B$19</formula>
-      <formula>$B$17</formula>
+  <conditionalFormatting sqref="B38:B43 B45:B48 B50:B54 B56:B61 B24:B29 B13:B16 B6:B11 B18:B22">
+    <cfRule type="cellIs" dxfId="29" priority="54" operator="between">
+      <formula>$B$20</formula>
+      <formula>$B$18</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:B10 B12:B15 B33:B37 B17:B21 B39:B42 B44:B48 B50:B55 B23:B28">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="between">
+  <conditionalFormatting sqref="B38:B43 B45:B48 B50:B54 B56:B61 B24:B29 B13:B16 B6:B11 B18:B22">
+    <cfRule type="cellIs" dxfId="28" priority="53" operator="between">
       <formula>0.99</formula>
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:B10 B12:B15 B33:B37 B17:B21 B39:B42 B44:B48 B50:B55 B23:B28">
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="between">
+  <conditionalFormatting sqref="B38:B43 B45:B48 B50:B54 B56:B61 B24:B29 B13:B16 B6:B11 B18:B22">
+    <cfRule type="cellIs" dxfId="27" priority="52" operator="between">
       <formula>0.79</formula>
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:B10 B12:B15 B33:B37 B17:B21 B39:B42 B44:B48 B50:B55 B23:B28">
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="lessThan">
+  <conditionalFormatting sqref="B38:B43 B45:B48 B50:B54 B56:B61 B24:B29 B13:B16 B6:B11 B18:B22">
+    <cfRule type="cellIs" dxfId="26" priority="51" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B58:B59">
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+  <conditionalFormatting sqref="B68:B69">
+    <cfRule type="cellIs" dxfId="25" priority="50" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B58:B59">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
+  <conditionalFormatting sqref="B68:B69">
+    <cfRule type="cellIs" dxfId="24" priority="49" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B58:B59">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="between">
-      <formula>$B$19</formula>
-      <formula>$B$17</formula>
+  <conditionalFormatting sqref="B68:B69">
+    <cfRule type="cellIs" dxfId="23" priority="48" operator="between">
+      <formula>$B$20</formula>
+      <formula>$B$18</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B58:B59">
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="between">
+  <conditionalFormatting sqref="B68:B69">
+    <cfRule type="cellIs" dxfId="22" priority="47" operator="between">
       <formula>0.99</formula>
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B58:B59">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="between">
+  <conditionalFormatting sqref="B68:B69">
+    <cfRule type="cellIs" dxfId="21" priority="46" operator="between">
       <formula>0.79</formula>
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B58:B59">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
+  <conditionalFormatting sqref="B68:B69">
+    <cfRule type="cellIs" dxfId="20" priority="45" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+  <conditionalFormatting sqref="B30">
+    <cfRule type="cellIs" dxfId="19" priority="44" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B56">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+  <conditionalFormatting sqref="B62">
+    <cfRule type="cellIs" dxfId="18" priority="43" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+  <conditionalFormatting sqref="B35">
+    <cfRule type="cellIs" dxfId="17" priority="42" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+  <conditionalFormatting sqref="B35">
+    <cfRule type="cellIs" dxfId="16" priority="41" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="between">
-      <formula>$B$19</formula>
-      <formula>$B$17</formula>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="cellIs" dxfId="15" priority="40" operator="between">
+      <formula>$B$20</formula>
+      <formula>$B$18</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="between">
+  <conditionalFormatting sqref="B35">
+    <cfRule type="cellIs" dxfId="14" priority="39" operator="between">
       <formula>0.99</formula>
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="between">
+  <conditionalFormatting sqref="B35">
+    <cfRule type="cellIs" dxfId="13" priority="38" operator="between">
       <formula>0.79</formula>
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
+  <conditionalFormatting sqref="B35">
+    <cfRule type="cellIs" dxfId="12" priority="37" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B57">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+  <conditionalFormatting sqref="B63:B67">
+    <cfRule type="cellIs" dxfId="11" priority="36" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B57">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+  <conditionalFormatting sqref="B63:B67">
+    <cfRule type="cellIs" dxfId="10" priority="35" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B57">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
-      <formula>$B$19</formula>
-      <formula>$B$17</formula>
+  <conditionalFormatting sqref="B63:B67">
+    <cfRule type="cellIs" dxfId="9" priority="34" operator="between">
+      <formula>$B$20</formula>
+      <formula>$B$18</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B57">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
+  <conditionalFormatting sqref="B63:B67">
+    <cfRule type="cellIs" dxfId="8" priority="33" operator="between">
       <formula>0.99</formula>
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B57">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+  <conditionalFormatting sqref="B63:B67">
+    <cfRule type="cellIs" dxfId="7" priority="32" operator="between">
       <formula>0.79</formula>
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B57">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="B63:B67">
+    <cfRule type="cellIs" dxfId="6" priority="31" operator="lessThan">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31:B34">
+    <cfRule type="cellIs" dxfId="5" priority="30" operator="equal">
+      <formula>100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31:B34">
+    <cfRule type="cellIs" dxfId="4" priority="29" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31:B34">
+    <cfRule type="cellIs" dxfId="3" priority="28" operator="between">
+      <formula>$B$20</formula>
+      <formula>$B$18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31:B34">
+    <cfRule type="cellIs" dxfId="2" priority="27" operator="between">
+      <formula>0.99</formula>
+      <formula>0.8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31:B34">
+    <cfRule type="cellIs" dxfId="1" priority="26" operator="between">
+      <formula>0.79</formula>
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31:B34">
+    <cfRule type="cellIs" dxfId="0" priority="25" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2969,7 +3356,7 @@
   <dimension ref="A2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2980,10 +3367,10 @@
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2991,7 +3378,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2999,31 +3386,31 @@
         <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -3032,17 +3419,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="45492d4d-eb53-4fd7-8815-9802ba598b13">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c494f3a6-0547-4149-a6d6-fbb0c535a61a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BBC74E8DCE70E84BBD871366DFA54C6D" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cd3cb58b6af65bc114028aad847fdade">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="45492d4d-eb53-4fd7-8815-9802ba598b13" xmlns:ns3="c494f3a6-0547-4149-a6d6-fbb0c535a61a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="443dfb89cbd5ad8f28d5213ec071e3ee" ns2:_="" ns3:_="">
     <xsd:import namespace="45492d4d-eb53-4fd7-8815-9802ba598b13"/>
@@ -3249,6 +3625,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="45492d4d-eb53-4fd7-8815-9802ba598b13">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c494f3a6-0547-4149-a6d6-fbb0c535a61a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3259,11 +3646,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AC7E76C-F8C5-480C-B35D-AC73615A3582}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3630A95F-7623-456D-8F06-8BD75A0E38DE}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3630A95F-7623-456D-8F06-8BD75A0E38DE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AC7E76C-F8C5-480C-B35D-AC73615A3582}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>